<commit_message>
Generate PCB project outputs
</commit_message>
<xml_diff>
--- a/Dub Siren PCB/Default Configuration/Project Outputs for Dub Siren PCB/BOM/BOM_PartType-Dub Siren PCB.xlsx
+++ b/Dub Siren PCB/Default Configuration/Project Outputs for Dub Siren PCB/BOM/BOM_PartType-Dub Siren PCB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="13395" windowHeight="11310"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="27795" windowHeight="17175"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_PartType-Dub Siren PCB" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
     <t>D1, D2</t>
   </si>
   <si>
-    <t>OVLBG4C7</t>
+    <t>WP424QR51WT/D-AMT</t>
   </si>
   <si>
     <t>LED 3mm</t>
@@ -103,7 +103,7 @@
     <t>R4, R5, R6, R7, R8, R9, R10, R11, R12</t>
   </si>
   <si>
-    <t>10k, RV09ACF-40</t>
+    <t>RV09AF-40-20K-B10K</t>
   </si>
   <si>
     <t>RV09ACF-40</t>

</xml_diff>